<commit_message>
Completing tests for broker performance
</commit_message>
<xml_diff>
--- a/Data/Buy-in calcs.xlsx
+++ b/Data/Buy-in calcs.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\Portfolio-management\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0861D0F-DEFC-4077-923D-BE9A464D01A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E568DC6A-567F-460E-B252-7BB5B3B38867}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13866" xr2:uid="{804967D6-7427-4AA1-91E1-1214B904BCF9}"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="14586" activeTab="1" xr2:uid="{804967D6-7427-4AA1-91E1-1214B904BCF9}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -67,10 +68,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="6">
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
-    <numFmt numFmtId="166" formatCode="0.0000"/>
-    <numFmt numFmtId="170" formatCode="#,##0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
+    <numFmt numFmtId="166" formatCode="#,##0.0000"/>
+    <numFmt numFmtId="167" formatCode="#,##0.00000"/>
+    <numFmt numFmtId="168" formatCode="#,##0.000000"/>
+    <numFmt numFmtId="170" formatCode="#,##0.0000000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -128,14 +132,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -144,6 +147,11 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="4" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -457,17 +465,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78B18952-1E91-41FE-A526-1E5441848050}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B6737E5-EE8F-4A0D-8F45-57704B771745}">
-  <dimension ref="B1:T37"/>
+  <dimension ref="B1:T46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N21" sqref="N21"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="I40" sqref="I40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="2" max="2" width="10.29296875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.29296875" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="9.234375" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="10.29296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -536,7 +558,7 @@
         <f>C3</f>
         <v>2</v>
       </c>
-      <c r="K3" s="1" t="str">
+      <c r="K3" s="16" t="str">
         <f t="shared" ref="K3:K9" si="0">IF(D3&lt;0,-(C3-J2)*D3,"")</f>
         <v/>
       </c>
@@ -545,7 +567,7 @@
         <v>2</v>
       </c>
       <c r="N3" s="1" t="str">
-        <f>IF(D3&lt;0,-(C3-M3)*D3,"")</f>
+        <f t="shared" ref="N3:N12" si="1">IF(D3&lt;0,-(C3-M3)*D3,"")</f>
         <v/>
       </c>
       <c r="P3" s="1">
@@ -561,7 +583,7 @@
         <v>2</v>
       </c>
       <c r="T3" t="str">
-        <f>IF(D3&lt;0,-(C3-S3)*D3,"")</f>
+        <f t="shared" ref="T3:T12" si="2">IF(D3&lt;0,-(C3-S3)*D3,"")</f>
         <v/>
       </c>
     </row>
@@ -580,18 +602,18 @@
         <v>7</v>
       </c>
       <c r="F4">
-        <f t="shared" ref="F4:F18" si="1">-C4*D4</f>
+        <f t="shared" ref="F4:F18" si="3">-C4*D4</f>
         <v>-8</v>
       </c>
       <c r="G4">
         <f>SUM($F$3:F4)</f>
         <v>-18</v>
       </c>
-      <c r="J4" s="1">
+      <c r="J4" s="14">
         <f>(J3*E3+MAX(0,D4)*C4)/E4</f>
         <v>2.5714285714285716</v>
       </c>
-      <c r="K4" s="1" t="str">
+      <c r="K4" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -600,7 +622,7 @@
         <v>2.5714285714285716</v>
       </c>
       <c r="N4" s="1" t="str">
-        <f>IF(D4&lt;0,-(C4-M4)*D4,"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="P4" s="1">
@@ -608,7 +630,7 @@
         <v>2</v>
       </c>
       <c r="Q4" s="1" t="str">
-        <f t="shared" ref="Q4:Q18" si="2">IF(D4&lt;0,-(C4-P4)*D4,"")</f>
+        <f t="shared" ref="Q4:Q18" si="4">IF(D4&lt;0,-(C4-P4)*D4,"")</f>
         <v/>
       </c>
       <c r="S4" s="1">
@@ -616,7 +638,7 @@
         <v>2.5714285714285716</v>
       </c>
       <c r="T4" t="str">
-        <f>IF(D4&lt;0,-(C4-S4)*D4,"")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -631,11 +653,11 @@
         <v>4</v>
       </c>
       <c r="E5">
-        <f t="shared" ref="E5:E9" si="3">E4+D5</f>
+        <f t="shared" ref="E5:E9" si="5">E4+D5</f>
         <v>11</v>
       </c>
       <c r="F5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>-28</v>
       </c>
       <c r="G5">
@@ -643,10 +665,10 @@
         <v>-46</v>
       </c>
       <c r="J5" s="4">
-        <f t="shared" ref="J5" si="4">(J4*E4+MAX(0,D5)*C5)/E5</f>
+        <f t="shared" ref="J5" si="6">(J4*E4+MAX(0,D5)*C5)/E5</f>
         <v>4.1818181818181817</v>
       </c>
-      <c r="K5" s="1" t="str">
+      <c r="K5" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -655,7 +677,7 @@
         <v>4.1818181818181817</v>
       </c>
       <c r="N5" s="1" t="str">
-        <f>IF(D5&lt;0,-(C5-M5)*D5,"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="P5" s="1">
@@ -663,7 +685,7 @@
         <v>2.5714285714285716</v>
       </c>
       <c r="Q5" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="S5" s="1">
@@ -671,7 +693,7 @@
         <v>4.1818181818181817</v>
       </c>
       <c r="T5" t="str">
-        <f>IF(D5&lt;0,-(C5-S5)*D5,"")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -686,11 +708,11 @@
         <v>-2</v>
       </c>
       <c r="E6">
+        <f t="shared" si="5"/>
+        <v>9</v>
+      </c>
+      <c r="F6">
         <f t="shared" si="3"/>
-        <v>9</v>
-      </c>
-      <c r="F6">
-        <f t="shared" si="1"/>
         <v>18</v>
       </c>
       <c r="G6">
@@ -701,7 +723,7 @@
         <f>(J5*E5+IF(D6&lt;0,J5,C6)*D6)/E6</f>
         <v>4.1818181818181825</v>
       </c>
-      <c r="K6" s="1">
+      <c r="K6" s="16">
         <f t="shared" si="0"/>
         <v>9.6363636363636367</v>
       </c>
@@ -710,7 +732,7 @@
         <v>4.1818181818181817</v>
       </c>
       <c r="N6" s="1">
-        <f>IF(D6&lt;0,-(C6-M6)*D6,"")</f>
+        <f t="shared" si="1"/>
         <v>9.6363636363636367</v>
       </c>
       <c r="P6" s="1">
@@ -718,7 +740,7 @@
         <v>4.1818181818181817</v>
       </c>
       <c r="Q6" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>9.6363636363636367</v>
       </c>
       <c r="S6" s="1">
@@ -726,7 +748,7 @@
         <v>4.1818181818181817</v>
       </c>
       <c r="T6" s="1">
-        <f>IF(D6&lt;0,-(C6-S6)*D6,"")</f>
+        <f t="shared" si="2"/>
         <v>9.6363636363636367</v>
       </c>
     </row>
@@ -741,22 +763,22 @@
         <v>3</v>
       </c>
       <c r="E7">
+        <f t="shared" si="5"/>
+        <v>12</v>
+      </c>
+      <c r="F7">
         <f t="shared" si="3"/>
-        <v>12</v>
-      </c>
-      <c r="F7">
-        <f t="shared" si="1"/>
         <v>-36</v>
       </c>
       <c r="G7">
         <f>SUM($F$3:F7)</f>
         <v>-64</v>
       </c>
-      <c r="J7" s="1">
-        <f t="shared" ref="J7:J9" si="5">(J6*E6+IF(D7&lt;0,J6,C7)*D7)/E7</f>
+      <c r="J7" s="15">
+        <f t="shared" ref="J7:J9" si="7">(J6*E6+IF(D7&lt;0,J6,C7)*D7)/E7</f>
         <v>6.1363636363636367</v>
       </c>
-      <c r="K7" s="1" t="str">
+      <c r="K7" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -765,7 +787,7 @@
         <v>5.8571428571428568</v>
       </c>
       <c r="N7" s="1" t="str">
-        <f>IF(D7&lt;0,-(C7-M7)*D7,"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="P7" s="1">
@@ -773,7 +795,7 @@
         <v>3.1111111111111112</v>
       </c>
       <c r="Q7" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="S7" s="1">
@@ -781,7 +803,7 @@
         <v>6.1363636363636358</v>
       </c>
       <c r="T7" t="str">
-        <f>IF(D7&lt;0,-(C7-S7)*D7,"")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -796,22 +818,22 @@
         <v>-7</v>
       </c>
       <c r="E8">
+        <f t="shared" si="5"/>
+        <v>5</v>
+      </c>
+      <c r="F8">
         <f t="shared" si="3"/>
-        <v>5</v>
-      </c>
-      <c r="F8">
-        <f t="shared" si="1"/>
         <v>119</v>
       </c>
       <c r="G8">
         <f>SUM($F$3:F8)</f>
         <v>55</v>
       </c>
-      <c r="J8" s="4">
-        <f t="shared" si="5"/>
+      <c r="J8" s="15">
+        <f t="shared" si="7"/>
         <v>6.1363636363636376</v>
       </c>
-      <c r="K8" s="1">
+      <c r="K8" s="16">
         <f t="shared" si="0"/>
         <v>76.045454545454547</v>
       </c>
@@ -820,7 +842,7 @@
         <v>5.8571428571428568</v>
       </c>
       <c r="N8" s="1">
-        <f>IF(D8&lt;0,-(C8-M8)*D8,"")</f>
+        <f t="shared" si="1"/>
         <v>78</v>
       </c>
       <c r="P8" s="1">
@@ -828,15 +850,15 @@
         <v>5.333333333333333</v>
       </c>
       <c r="Q8" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>81.666666666666671</v>
       </c>
-      <c r="S8" s="1">
+      <c r="S8" s="14">
         <f>S7</f>
         <v>6.1363636363636358</v>
       </c>
       <c r="T8" s="1">
-        <f>IF(D8&lt;0,-(C8-S8)*D8,"")</f>
+        <f t="shared" si="2"/>
         <v>76.045454545454547</v>
       </c>
     </row>
@@ -851,22 +873,22 @@
         <v>2</v>
       </c>
       <c r="E9">
+        <f t="shared" si="5"/>
+        <v>7</v>
+      </c>
+      <c r="F9">
         <f t="shared" si="3"/>
-        <v>7</v>
-      </c>
-      <c r="F9">
-        <f t="shared" si="1"/>
         <v>-36</v>
       </c>
       <c r="G9">
         <f>SUM($F$3:F9)</f>
         <v>19</v>
       </c>
-      <c r="J9" s="4">
-        <f t="shared" si="5"/>
+      <c r="J9" s="15">
+        <f t="shared" si="7"/>
         <v>9.5259740259740262</v>
       </c>
-      <c r="K9" s="1" t="str">
+      <c r="K9" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -876,7 +898,7 @@
         <v>7.375</v>
       </c>
       <c r="N9" s="1" t="str">
-        <f>IF(D9&lt;0,-(C9-M9)*D9,"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="P9" s="1">
@@ -884,7 +906,7 @@
         <v>-11</v>
       </c>
       <c r="Q9" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="S9" s="1">
@@ -892,7 +914,7 @@
         <v>6.1363636363636358</v>
       </c>
       <c r="T9" s="1" t="str">
-        <f>IF(D9&lt;0,-(C9-S9)*D9,"")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -907,26 +929,26 @@
         <v>-7</v>
       </c>
       <c r="E10">
-        <f t="shared" ref="E10" si="6">E9+D10</f>
+        <f t="shared" ref="E10" si="8">E9+D10</f>
         <v>0</v>
       </c>
       <c r="F10">
-        <f t="shared" ref="F10" si="7">-C10*D10</f>
+        <f t="shared" ref="F10" si="9">-C10*D10</f>
         <v>133</v>
       </c>
-      <c r="G10" s="7">
+      <c r="G10" s="6">
         <f>SUM($F$3:F10)</f>
         <v>152</v>
       </c>
       <c r="J10" s="4" t="e">
-        <f t="shared" ref="J10" si="8">(J9*E9+IF(D10&lt;0,J9,C10)*D10)/E10</f>
+        <f t="shared" ref="J10" si="10">(J9*E9+IF(D10&lt;0,J9,C10)*D10)/E10</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="K10" s="1">
-        <f t="shared" ref="K10" si="9">IF(D10&lt;0,-(C10-J9)*D10,"")</f>
+      <c r="K10" s="16">
+        <f t="shared" ref="K10" si="11">IF(D10&lt;0,-(C10-J9)*D10,"")</f>
         <v>66.318181818181813</v>
       </c>
-      <c r="L10" s="6">
+      <c r="L10" s="18">
         <f>SUM(K3:K10)</f>
         <v>152</v>
       </c>
@@ -935,7 +957,7 @@
         <v>7.375</v>
       </c>
       <c r="N10" s="1">
-        <f>IF(D10&lt;0,-(C10-M10)*D10,"")</f>
+        <f t="shared" si="1"/>
         <v>81.375</v>
       </c>
       <c r="P10" s="1">
@@ -943,7 +965,7 @@
         <v>-2.7142857142857144</v>
       </c>
       <c r="Q10" s="1">
-        <f t="shared" ref="Q10" si="10">IF(D10&lt;0,-(C10-P10)*D10,"")</f>
+        <f t="shared" ref="Q10" si="12">IF(D10&lt;0,-(C10-P10)*D10,"")</f>
         <v>152</v>
       </c>
       <c r="S10" s="1">
@@ -951,7 +973,7 @@
         <v>6.1363636363636358</v>
       </c>
       <c r="T10" s="1">
-        <f>IF(D10&lt;0,-(C10-S10)*D10,"")</f>
+        <f t="shared" si="2"/>
         <v>90.045454545454547</v>
       </c>
     </row>
@@ -966,11 +988,11 @@
         <v>-9</v>
       </c>
       <c r="E11">
-        <f t="shared" ref="E11:E18" si="11">E10+D11</f>
+        <f t="shared" ref="E11:E18" si="13">E10+D11</f>
         <v>-9</v>
       </c>
       <c r="F11">
-        <f t="shared" ref="F11" si="12">-C11*D11</f>
+        <f t="shared" ref="F11" si="14">-C11*D11</f>
         <v>180</v>
       </c>
       <c r="G11">
@@ -981,14 +1003,14 @@
         <f>C11</f>
         <v>20</v>
       </c>
-      <c r="K11" s="1"/>
+      <c r="K11" s="16"/>
       <c r="L11" s="1"/>
       <c r="M11" s="1">
         <f>-SUMIF($D$3:D11,"&gt;0",$F$3:F11)/SUMIF($D$3:D11,"&gt;0",$D$3:D11)</f>
         <v>7.375</v>
       </c>
       <c r="N11" s="1">
-        <f>IF(D11&lt;0,-(C11-M11)*D11,"")</f>
+        <f t="shared" si="1"/>
         <v>113.625</v>
       </c>
       <c r="P11" s="1" t="e">
@@ -996,7 +1018,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="Q11" s="1" t="e">
-        <f t="shared" ref="Q11" si="13">IF(D11&lt;0,-(C11-P11)*D11,"")</f>
+        <f t="shared" ref="Q11" si="15">IF(D11&lt;0,-(C11-P11)*D11,"")</f>
         <v>#DIV/0!</v>
       </c>
       <c r="S11" s="1">
@@ -1004,7 +1026,7 @@
         <v>6.1363636363636358</v>
       </c>
       <c r="T11" s="1">
-        <f>IF(D11&lt;0,-(C11-S11)*D11,"")</f>
+        <f t="shared" si="2"/>
         <v>124.77272727272727</v>
       </c>
     </row>
@@ -1019,11 +1041,11 @@
         <v>-11</v>
       </c>
       <c r="E12">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>-20</v>
       </c>
       <c r="F12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>198</v>
       </c>
       <c r="G12">
@@ -1034,7 +1056,7 @@
         <f>(J11*E11+IF(D12&gt;0,J11,C12)*D12)/E12</f>
         <v>18.899999999999999</v>
       </c>
-      <c r="K12" s="1" t="str">
+      <c r="K12" s="16" t="str">
         <f>IF(D12&gt;0,-(C12-J11)*D12,"")</f>
         <v/>
       </c>
@@ -1044,12 +1066,12 @@
         <v>7.375</v>
       </c>
       <c r="N12" s="1">
-        <f>IF(D12&lt;0,-(C12-M12)*D12,"")</f>
+        <f t="shared" si="1"/>
         <v>116.875</v>
       </c>
       <c r="P12" s="1"/>
       <c r="Q12" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>198</v>
       </c>
       <c r="S12" s="1">
@@ -1057,7 +1079,7 @@
         <v>6.1363636363636358</v>
       </c>
       <c r="T12" s="1">
-        <f>IF(D12&lt;0,-(C12-S12)*D12,"")</f>
+        <f t="shared" si="2"/>
         <v>130.5</v>
       </c>
     </row>
@@ -1072,11 +1094,11 @@
         <v>5</v>
       </c>
       <c r="E13">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>-15</v>
       </c>
       <c r="F13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>-120</v>
       </c>
       <c r="G13">
@@ -1087,7 +1109,7 @@
         <f>(J12*E12+IF(D13&gt;0,J12,C13)*D13)/E13</f>
         <v>18.899999999999999</v>
       </c>
-      <c r="K13" s="1">
+      <c r="K13" s="16">
         <f>IF(D13&gt;0,-(C13-J12)*D13,"")</f>
         <v>-25.500000000000007</v>
       </c>
@@ -1096,7 +1118,7 @@
       <c r="N13" s="1"/>
       <c r="P13" s="1"/>
       <c r="Q13" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="S13" s="1"/>
@@ -1113,14 +1135,14 @@
         <v>15</v>
       </c>
       <c r="E14">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="F14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>-180</v>
       </c>
-      <c r="G14" s="9">
+      <c r="G14" s="8">
         <f>SUM($F$11:F14)</f>
         <v>78</v>
       </c>
@@ -1128,11 +1150,11 @@
         <f>(J13*E13+IF(D14&gt;0,J13,C14)*D14)/E14</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="K14" s="1">
+      <c r="K14" s="16">
         <f>IF(D14&gt;0,-(C14-J13)*D14,"")</f>
         <v>103.49999999999997</v>
       </c>
-      <c r="L14" s="8">
+      <c r="L14" s="7">
         <f>SUM(K12:K14)</f>
         <v>77.999999999999972</v>
       </c>
@@ -1140,28 +1162,28 @@
       <c r="N14" s="1"/>
       <c r="P14" s="1"/>
       <c r="Q14" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="S14" s="1"/>
       <c r="T14" s="1"/>
     </row>
-    <row r="15" spans="2:20" s="11" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="B15" s="10">
+    <row r="15" spans="2:20" s="10" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="B15" s="9">
         <v>45214</v>
       </c>
-      <c r="C15" s="11">
+      <c r="C15" s="10">
         <v>18</v>
       </c>
-      <c r="D15" s="11">
+      <c r="D15" s="10">
         <v>5</v>
       </c>
       <c r="E15">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>5</v>
       </c>
-      <c r="F15" s="11">
-        <f t="shared" si="1"/>
+      <c r="F15" s="10">
+        <f t="shared" si="3"/>
         <v>-90</v>
       </c>
       <c r="G15">
@@ -1172,37 +1194,37 @@
         <f>C15</f>
         <v>18</v>
       </c>
-      <c r="K15" s="1" t="str">
-        <f t="shared" ref="K15:K18" si="14">IF(D15&lt;0,-(C15-J14)*D15,"")</f>
-        <v/>
-      </c>
-      <c r="L15" s="12"/>
-      <c r="M15" s="12"/>
-      <c r="N15" s="12"/>
-      <c r="P15" s="12"/>
-      <c r="Q15" s="12" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="S15" s="12"/>
-      <c r="T15" s="12"/>
-    </row>
-    <row r="16" spans="2:20" s="11" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="B16" s="10">
+      <c r="K15" s="16" t="str">
+        <f t="shared" ref="K15:K18" si="16">IF(D15&lt;0,-(C15-J14)*D15,"")</f>
+        <v/>
+      </c>
+      <c r="L15" s="11"/>
+      <c r="M15" s="11"/>
+      <c r="N15" s="11"/>
+      <c r="P15" s="11"/>
+      <c r="Q15" s="11" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="S15" s="11"/>
+      <c r="T15" s="11"/>
+    </row>
+    <row r="16" spans="2:20" s="10" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="B16" s="9">
         <v>45219</v>
       </c>
-      <c r="C16" s="11">
+      <c r="C16" s="10">
         <v>11</v>
       </c>
-      <c r="D16" s="11">
+      <c r="D16" s="10">
         <v>-2</v>
       </c>
       <c r="E16">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>3</v>
       </c>
-      <c r="F16" s="11">
-        <f t="shared" si="1"/>
+      <c r="F16" s="10">
+        <f t="shared" si="3"/>
         <v>22</v>
       </c>
       <c r="G16">
@@ -1210,40 +1232,40 @@
         <v>-68</v>
       </c>
       <c r="J16" s="4">
-        <f t="shared" ref="J15:J18" si="15">(J15*E15+IF(D16&lt;0,J15,C16)*D16)/E16</f>
+        <f t="shared" ref="J16:J18" si="17">(J15*E15+IF(D16&lt;0,J15,C16)*D16)/E16</f>
         <v>18</v>
       </c>
-      <c r="K16" s="1">
-        <f t="shared" si="14"/>
+      <c r="K16" s="16">
+        <f t="shared" si="16"/>
         <v>-14</v>
       </c>
-      <c r="L16" s="12"/>
-      <c r="M16" s="12"/>
-      <c r="N16" s="12"/>
-      <c r="P16" s="12"/>
-      <c r="Q16" s="12">
-        <f t="shared" si="2"/>
+      <c r="L16" s="11"/>
+      <c r="M16" s="11"/>
+      <c r="N16" s="11"/>
+      <c r="P16" s="11"/>
+      <c r="Q16" s="11">
+        <f t="shared" si="4"/>
         <v>22</v>
       </c>
-      <c r="S16" s="12"/>
-      <c r="T16" s="12"/>
-    </row>
-    <row r="17" spans="2:20" s="11" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="B17" s="10">
+      <c r="S16" s="11"/>
+      <c r="T16" s="11"/>
+    </row>
+    <row r="17" spans="2:20" s="10" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="B17" s="9">
         <v>45245</v>
       </c>
-      <c r="C17" s="11">
+      <c r="C17" s="10">
         <v>23</v>
       </c>
-      <c r="D17" s="11">
+      <c r="D17" s="10">
         <v>3</v>
       </c>
       <c r="E17">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>6</v>
       </c>
-      <c r="F17" s="11">
-        <f t="shared" si="1"/>
+      <c r="F17" s="10">
+        <f t="shared" si="3"/>
         <v>-69</v>
       </c>
       <c r="G17">
@@ -1251,67 +1273,67 @@
         <v>-137</v>
       </c>
       <c r="J17" s="4">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>20.5</v>
       </c>
-      <c r="K17" s="1" t="str">
-        <f t="shared" si="14"/>
-        <v/>
-      </c>
-      <c r="L17" s="12"/>
-      <c r="M17" s="12"/>
-      <c r="N17" s="12"/>
-      <c r="P17" s="12"/>
-      <c r="Q17" s="12" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="S17" s="12"/>
-      <c r="T17" s="12"/>
-    </row>
-    <row r="18" spans="2:20" s="11" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="B18" s="10">
+      <c r="K17" s="16" t="str">
+        <f t="shared" si="16"/>
+        <v/>
+      </c>
+      <c r="L17" s="11"/>
+      <c r="M17" s="11"/>
+      <c r="N17" s="11"/>
+      <c r="P17" s="11"/>
+      <c r="Q17" s="11" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="S17" s="11"/>
+      <c r="T17" s="11"/>
+    </row>
+    <row r="18" spans="2:20" s="10" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="B18" s="9">
         <v>45261</v>
       </c>
-      <c r="C18" s="11">
+      <c r="C18" s="10">
         <v>21</v>
       </c>
-      <c r="D18" s="11">
+      <c r="D18" s="10">
         <v>-6</v>
       </c>
       <c r="E18">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="F18" s="11">
-        <f t="shared" si="1"/>
+      <c r="F18" s="10">
+        <f t="shared" si="3"/>
         <v>126</v>
       </c>
-      <c r="G18" s="14">
+      <c r="G18" s="13">
         <f>SUM($F$15:F18)</f>
         <v>-11</v>
       </c>
       <c r="J18" s="4" t="e">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>#DIV/0!</v>
       </c>
       <c r="K18" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>3</v>
       </c>
-      <c r="L18" s="13">
+      <c r="L18" s="12">
         <f>SUM(K16:K18)</f>
         <v>-11</v>
       </c>
-      <c r="M18" s="12"/>
-      <c r="N18" s="12"/>
-      <c r="P18" s="12"/>
-      <c r="Q18" s="12">
-        <f t="shared" si="2"/>
+      <c r="M18" s="11"/>
+      <c r="N18" s="11"/>
+      <c r="P18" s="11"/>
+      <c r="Q18" s="11">
+        <f t="shared" si="4"/>
         <v>126</v>
       </c>
-      <c r="S18" s="12"/>
-      <c r="T18" s="12"/>
+      <c r="S18" s="11"/>
+      <c r="T18" s="11"/>
     </row>
     <row r="19" spans="2:20" x14ac:dyDescent="0.5">
       <c r="F19" s="2">
@@ -1373,75 +1395,75 @@
         <v>45069</v>
       </c>
       <c r="C24">
-        <f t="shared" ref="C24:E24" si="16">C7</f>
+        <f t="shared" ref="C24:E24" si="18">C7</f>
         <v>12</v>
       </c>
       <c r="D24">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>3</v>
       </c>
       <c r="E24">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>12</v>
       </c>
       <c r="F24">
-        <f t="shared" ref="F24:F26" si="17">-C24*D24</f>
+        <f t="shared" ref="F24:F26" si="19">-C24*D24</f>
         <v>-36</v>
       </c>
       <c r="J24" s="4">
-        <f t="shared" ref="J24:J26" si="18">(J23*E23+IF(D24&lt;0,J23,C24)*D24)/E24</f>
+        <f t="shared" ref="J24:J26" si="20">(J23*E23+IF(D24&lt;0,J23,C24)*D24)/E24</f>
         <v>9.75</v>
       </c>
     </row>
     <row r="25" spans="2:20" x14ac:dyDescent="0.5">
       <c r="B25" s="3">
-        <f t="shared" ref="B25:E25" si="19">B8</f>
+        <f t="shared" ref="B25:E25" si="21">B8</f>
         <v>45087</v>
       </c>
       <c r="C25">
+        <f t="shared" si="21"/>
+        <v>17</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="21"/>
+        <v>-7</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="21"/>
+        <v>5</v>
+      </c>
+      <c r="F25">
         <f t="shared" si="19"/>
-        <v>17</v>
-      </c>
-      <c r="D25">
-        <f t="shared" si="19"/>
-        <v>-7</v>
-      </c>
-      <c r="E25">
-        <f t="shared" si="19"/>
-        <v>5</v>
-      </c>
-      <c r="F25">
-        <f t="shared" si="17"/>
         <v>119</v>
       </c>
       <c r="J25" s="4">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>9.75</v>
       </c>
     </row>
     <row r="26" spans="2:20" x14ac:dyDescent="0.5">
       <c r="B26" s="3">
-        <f t="shared" ref="B26:E26" si="20">B9</f>
+        <f t="shared" ref="B26:E26" si="22">B9</f>
         <v>45129</v>
       </c>
       <c r="C26">
+        <f t="shared" si="22"/>
+        <v>18</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="22"/>
+        <v>2</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="22"/>
+        <v>7</v>
+      </c>
+      <c r="F26">
+        <f t="shared" si="19"/>
+        <v>-36</v>
+      </c>
+      <c r="J26" s="15">
         <f t="shared" si="20"/>
-        <v>18</v>
-      </c>
-      <c r="D26">
-        <f t="shared" si="20"/>
-        <v>2</v>
-      </c>
-      <c r="E26">
-        <f t="shared" si="20"/>
-        <v>7</v>
-      </c>
-      <c r="F26">
-        <f t="shared" si="17"/>
-        <v>-36</v>
-      </c>
-      <c r="J26" s="4">
-        <f t="shared" si="18"/>
         <v>12.107142857142858</v>
       </c>
     </row>
@@ -1457,23 +1479,23 @@
     </row>
     <row r="30" spans="2:20" x14ac:dyDescent="0.5">
       <c r="B30" s="3">
-        <f>B3</f>
+        <f t="shared" ref="B30:B36" si="23">B3</f>
         <v>44927</v>
       </c>
       <c r="C30" s="1">
-        <f>C3/G30</f>
+        <f t="shared" ref="C30:C36" si="24">C3/G30</f>
         <v>1.8181818181818181</v>
       </c>
       <c r="D30">
-        <f>D3</f>
+        <f t="shared" ref="D30:E36" si="25">D3</f>
         <v>5</v>
       </c>
       <c r="E30">
-        <f>E3</f>
+        <f t="shared" si="25"/>
         <v>5</v>
       </c>
       <c r="F30" s="1">
-        <f t="shared" ref="F30:F36" si="21">-C30*D30</f>
+        <f t="shared" ref="F30:F36" si="26">-C30*D30</f>
         <v>-9.0909090909090899</v>
       </c>
       <c r="G30">
@@ -1493,27 +1515,27 @@
     </row>
     <row r="31" spans="2:20" x14ac:dyDescent="0.5">
       <c r="B31" s="3">
-        <f>B4</f>
+        <f t="shared" si="23"/>
         <v>44972</v>
       </c>
       <c r="C31" s="1">
-        <f>C4/G31</f>
+        <f t="shared" si="24"/>
         <v>3.6363636363636362</v>
       </c>
       <c r="D31">
-        <f>D4</f>
+        <f t="shared" si="25"/>
         <v>2</v>
       </c>
       <c r="E31">
-        <f>E4</f>
+        <f t="shared" si="25"/>
         <v>7</v>
       </c>
       <c r="F31" s="1">
-        <f t="shared" si="21"/>
+        <f t="shared" si="26"/>
         <v>-7.2727272727272725</v>
       </c>
       <c r="G31">
-        <f t="shared" ref="G31:G36" si="22">VLOOKUP(B31,$N$30:$O$32,2,1)</f>
+        <f t="shared" ref="G31:G36" si="27">VLOOKUP(B31,$N$30:$O$32,2,1)</f>
         <v>1.1000000000000001</v>
       </c>
       <c r="J31" s="1">
@@ -1529,31 +1551,31 @@
     </row>
     <row r="32" spans="2:20" x14ac:dyDescent="0.5">
       <c r="B32" s="3">
-        <f>B5</f>
+        <f t="shared" si="23"/>
         <v>44997</v>
       </c>
       <c r="C32" s="1">
-        <f>C5/G32</f>
+        <f t="shared" si="24"/>
         <v>6.0869565217391308</v>
       </c>
       <c r="D32">
-        <f>D5</f>
+        <f t="shared" si="25"/>
         <v>4</v>
       </c>
       <c r="E32">
-        <f>E5</f>
+        <f t="shared" si="25"/>
         <v>11</v>
       </c>
       <c r="F32" s="1">
-        <f t="shared" si="21"/>
+        <f t="shared" si="26"/>
         <v>-24.347826086956523</v>
       </c>
       <c r="G32">
-        <f t="shared" si="22"/>
+        <f t="shared" si="27"/>
         <v>1.1499999999999999</v>
       </c>
       <c r="J32" s="4">
-        <f t="shared" ref="J32:J36" si="23">(J31*E31+MAX(0,D32)*C32)/E32</f>
+        <f t="shared" ref="J32" si="28">(J31*E31+MAX(0,D32)*C32)/E32</f>
         <v>3.7010420409629901</v>
       </c>
       <c r="N32" s="3">
@@ -1565,27 +1587,27 @@
     </row>
     <row r="33" spans="2:10" x14ac:dyDescent="0.5">
       <c r="B33" s="3">
-        <f>B6</f>
+        <f t="shared" si="23"/>
         <v>45021</v>
       </c>
       <c r="C33" s="1">
-        <f>C6/G33</f>
+        <f t="shared" si="24"/>
         <v>7.8260869565217401</v>
       </c>
       <c r="D33">
-        <f>D6</f>
+        <f t="shared" si="25"/>
         <v>-2</v>
       </c>
       <c r="E33">
-        <f>E6</f>
+        <f t="shared" si="25"/>
         <v>9</v>
       </c>
       <c r="F33" s="1">
-        <f t="shared" si="21"/>
+        <f t="shared" si="26"/>
         <v>15.65217391304348</v>
       </c>
       <c r="G33">
-        <f t="shared" si="22"/>
+        <f t="shared" si="27"/>
         <v>1.1499999999999999</v>
       </c>
       <c r="J33" s="4">
@@ -1595,99 +1617,173 @@
     </row>
     <row r="34" spans="2:10" x14ac:dyDescent="0.5">
       <c r="B34" s="3">
-        <f>B7</f>
+        <f t="shared" si="23"/>
         <v>45069</v>
       </c>
       <c r="C34" s="1">
-        <f>C7/G34</f>
+        <f t="shared" si="24"/>
         <v>9.6</v>
       </c>
       <c r="D34">
-        <f>D7</f>
+        <f t="shared" si="25"/>
         <v>3</v>
       </c>
       <c r="E34">
-        <f>E7</f>
+        <f t="shared" si="25"/>
         <v>12</v>
       </c>
       <c r="F34" s="1">
-        <f t="shared" si="21"/>
+        <f t="shared" si="26"/>
         <v>-28.799999999999997</v>
       </c>
       <c r="G34">
-        <f t="shared" si="22"/>
+        <f t="shared" si="27"/>
         <v>1.25</v>
       </c>
       <c r="J34" s="4">
-        <f t="shared" ref="J34:J37" si="24">(J33*E33+IF(D34&lt;0,J33,C34)*D34)/E34</f>
+        <f t="shared" ref="J34:J37" si="29">(J33*E33+IF(D34&lt;0,J33,C34)*D34)/E34</f>
         <v>5.1757815307222428</v>
       </c>
     </row>
     <row r="35" spans="2:10" x14ac:dyDescent="0.5">
       <c r="B35" s="3">
-        <f>B8</f>
+        <f t="shared" si="23"/>
         <v>45087</v>
       </c>
       <c r="C35" s="1">
-        <f>C8/G35</f>
+        <f t="shared" si="24"/>
         <v>13.6</v>
       </c>
       <c r="D35">
-        <f>D8</f>
+        <f t="shared" si="25"/>
         <v>-7</v>
       </c>
       <c r="E35">
-        <f>E8</f>
+        <f t="shared" si="25"/>
         <v>5</v>
       </c>
       <c r="F35" s="1">
-        <f t="shared" si="21"/>
+        <f t="shared" si="26"/>
         <v>95.2</v>
       </c>
       <c r="G35">
-        <f t="shared" si="22"/>
+        <f t="shared" si="27"/>
         <v>1.25</v>
       </c>
       <c r="J35" s="4">
-        <f t="shared" si="24"/>
+        <f t="shared" si="29"/>
         <v>5.1757815307222419</v>
       </c>
     </row>
     <row r="36" spans="2:10" x14ac:dyDescent="0.5">
       <c r="B36" s="3">
-        <f>B9</f>
+        <f t="shared" si="23"/>
         <v>45129</v>
       </c>
       <c r="C36" s="1">
-        <f>C9/G36</f>
+        <f t="shared" si="24"/>
         <v>14.4</v>
       </c>
       <c r="D36">
-        <f>D9</f>
+        <f t="shared" si="25"/>
         <v>2</v>
       </c>
       <c r="E36">
-        <f>E9</f>
+        <f t="shared" si="25"/>
         <v>7</v>
       </c>
       <c r="F36" s="1">
-        <f t="shared" si="21"/>
+        <f t="shared" si="26"/>
         <v>-28.8</v>
       </c>
       <c r="G36">
-        <f t="shared" si="22"/>
+        <f t="shared" si="27"/>
         <v>1.25</v>
       </c>
       <c r="J36" s="4">
-        <f t="shared" si="24"/>
+        <f t="shared" si="29"/>
         <v>7.8112725219444581</v>
       </c>
     </row>
     <row r="37" spans="2:10" x14ac:dyDescent="0.5">
       <c r="J37" s="4" t="e">
-        <f t="shared" si="24"/>
+        <f t="shared" si="29"/>
         <v>#DIV/0!</v>
       </c>
+    </row>
+    <row r="39" spans="2:10" x14ac:dyDescent="0.5">
+      <c r="H39" s="3">
+        <f>B30</f>
+        <v>44927</v>
+      </c>
+      <c r="I39" s="15">
+        <f>J30</f>
+        <v>1.8181818181818181</v>
+      </c>
+    </row>
+    <row r="40" spans="2:10" x14ac:dyDescent="0.5">
+      <c r="H40" s="3">
+        <f t="shared" ref="H40:H46" si="30">B31</f>
+        <v>44972</v>
+      </c>
+      <c r="I40" s="17">
+        <f t="shared" ref="I40:I46" si="31">J31</f>
+        <v>2.3376623376623376</v>
+      </c>
+    </row>
+    <row r="41" spans="2:10" x14ac:dyDescent="0.5">
+      <c r="H41" s="3">
+        <f t="shared" si="30"/>
+        <v>44997</v>
+      </c>
+      <c r="I41" s="15">
+        <f t="shared" si="31"/>
+        <v>3.7010420409629901</v>
+      </c>
+    </row>
+    <row r="42" spans="2:10" x14ac:dyDescent="0.5">
+      <c r="H42" s="3">
+        <f t="shared" si="30"/>
+        <v>45021</v>
+      </c>
+      <c r="I42" s="15">
+        <f t="shared" si="31"/>
+        <v>3.7010420409629905</v>
+      </c>
+    </row>
+    <row r="43" spans="2:10" x14ac:dyDescent="0.5">
+      <c r="H43" s="3">
+        <f t="shared" si="30"/>
+        <v>45069</v>
+      </c>
+      <c r="I43" s="15">
+        <f t="shared" si="31"/>
+        <v>5.1757815307222428</v>
+      </c>
+    </row>
+    <row r="44" spans="2:10" x14ac:dyDescent="0.5">
+      <c r="H44" s="3">
+        <f t="shared" si="30"/>
+        <v>45087</v>
+      </c>
+      <c r="I44" s="15">
+        <f t="shared" si="31"/>
+        <v>5.1757815307222419</v>
+      </c>
+    </row>
+    <row r="45" spans="2:10" x14ac:dyDescent="0.5">
+      <c r="H45" s="3">
+        <f t="shared" si="30"/>
+        <v>45129</v>
+      </c>
+      <c r="I45" s="15">
+        <f t="shared" si="31"/>
+        <v>7.8112725219444581</v>
+      </c>
+    </row>
+    <row r="46" spans="2:10" x14ac:dyDescent="0.5">
+      <c r="H46" s="3"/>
+      <c r="I46" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>